<commit_message>
from PC May04 2018
</commit_message>
<xml_diff>
--- a/python/data/iterate_test.xlsx
+++ b/python/data/iterate_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>date</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>2018-01-22</t>
-  </si>
-  <si>
-    <t>2018-03-08</t>
   </si>
   <si>
     <t>5.000000</t>
@@ -431,7 +428,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -450,7 +447,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -458,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -466,7 +463,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -474,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -482,7 +479,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -490,7 +487,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -498,7 +495,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -506,7 +503,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -514,7 +511,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -522,7 +519,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -530,7 +527,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -538,7 +535,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -546,7 +543,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -554,7 +551,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -562,14 +559,6 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>